<commit_message>
README.md 更新、DEC Module を追加
</commit_message>
<xml_diff>
--- a/htdocs/px-files/sitemaps/sitemap.xlsx
+++ b/htdocs/px-files/sitemaps/sitemap.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25725"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620"/>
   </bookViews>
   <sheets>
-    <sheet name="sitemap" sheetId="1" r:id="rId4"/>
+    <sheet name="sitemap" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>row_definition=8&amp;row_data_start=9&amp;skip_empty_col=20&amp;version=2.0.1</t>
   </si>
@@ -126,57 +130,60 @@
   </si>
   <si>
     <t>EndOfData</t>
+  </si>
+  <si>
+    <t>Edit Sample</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>/edit_sample/</t>
+    <phoneticPr fontId="5"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="メイリオ"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="8"/>
       <color rgb="FF333333"/>
       <name val="メイリオ"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="24"/>
       <color rgb="FF000000"/>
       <name val="メイリオ"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="メイリオ"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="8"/>
       <color rgb="FF000000"/>
+      <name val="メイリオ"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="メイリオ"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="メイリオ"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="メイリオ"/>
     </font>
   </fonts>
@@ -185,10 +192,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -204,19 +208,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFcccccc"/>
+        <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFdddddd"/>
+        <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="4">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -230,13 +240,14 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFdddddd"/>
+        <color rgb="FFDDDDDD"/>
       </left>
       <right style="thin">
-        <color rgb="FFdddddd"/>
+        <color rgb="FFDDDDDD"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -244,13 +255,14 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF666666"/>
       </left>
       <right style="thin">
-        <color rgb="FFdddddd"/>
+        <color rgb="FFDDDDDD"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -258,48 +270,36 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="5" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="5" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -589,42 +589,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:S12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.625" defaultRowHeight="19" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8" customWidth="true" style="0"/>
-    <col min="2" max="2" width="3" customWidth="true" style="0"/>
-    <col min="3" max="3" width="3" customWidth="true" style="0"/>
-    <col min="4" max="4" width="3" customWidth="true" style="0"/>
-    <col min="5" max="5" width="3" customWidth="true" style="0"/>
-    <col min="6" max="6" width="20" customWidth="true" style="0"/>
-    <col min="7" max="7" width="2" customWidth="true" style="0"/>
-    <col min="8" max="8" width="2" customWidth="true" style="0"/>
-    <col min="9" max="9" width="2" customWidth="true" style="0"/>
-    <col min="10" max="10" width="2" customWidth="true" style="0"/>
-    <col min="11" max="11" width="40" customWidth="true" style="0"/>
-    <col min="12" max="12" width="20" customWidth="true" style="0"/>
-    <col min="13" max="13" width="3" customWidth="true" style="0"/>
-    <col min="14" max="14" width="9" customWidth="true" style="0"/>
-    <col min="17" max="17" width="30" customWidth="true" style="0"/>
-    <col min="16" max="16" width="30" customWidth="true" style="0"/>
-    <col min="15" max="15" width="3" customWidth="true" style="0"/>
-    <col min="18" max="18" width="3" customWidth="true" style="0"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="5" width="3" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="10" width="2" customWidth="1"/>
+    <col min="11" max="11" width="40" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
+    <col min="13" max="13" width="3" customWidth="1"/>
+    <col min="14" max="14" width="9" customWidth="1"/>
+    <col min="15" max="15" width="3" customWidth="1"/>
+    <col min="16" max="17" width="30" customWidth="1"/>
+    <col min="18" max="18" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" customHeight="1" ht="10">
+    <row r="1" spans="1:19" ht="10" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +637,7 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" ht="37">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -661,13 +651,13 @@
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
       <c r="G7" s="3" t="s">
         <v>5</v>
       </c>
@@ -712,13 +702,13 @@
       <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
       <c r="G8" s="5" t="s">
         <v>20</v>
       </c>
@@ -788,45 +778,70 @@
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
     </row>
-    <row r="12" spans="1:19" customHeight="1" ht="5">
-      <c r="A12" s="9" t="s">
+    <row r="10" spans="1:19">
+      <c r="A10" s="4"/>
+      <c r="C10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4">
+        <v>1</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="4">
+        <v>1</v>
+      </c>
+      <c r="S10" s="4"/>
+    </row>
+    <row r="13" spans="1:19" ht="5" customHeight="1">
+      <c r="A13" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <mergeCells>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="2">
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="B8:F8"/>
   </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <phoneticPr fontId="5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>